<commit_message>
Before changes to fast string index.
</commit_message>
<xml_diff>
--- a/traitsnew.xlsx
+++ b/traitsnew.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="375" windowWidth="18870" windowHeight="8340"/>
+    <workbookView xWindow="360" yWindow="375" windowWidth="18870" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -55,7 +55,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t>Uživatel systému Windows:</t>
         </r>
@@ -64,7 +65,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
 SK: Domena je registrovana (aaaskoda.sk)
@@ -107,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Trait ID</t>
   </si>
@@ -121,30 +123,15 @@
     <t>Parking</t>
   </si>
   <si>
-    <t>Když se jedná o doménu, která obsahuje webove stranky providera nebo se na strankách pracuje</t>
-  </si>
-  <si>
-    <t>Doména existuje, ale nejdou stáhnout žádné stránky.</t>
-  </si>
-  <si>
     <t>More</t>
   </si>
   <si>
     <t>Forwarding</t>
   </si>
   <si>
-    <t>Je tam forwarding, Je potreba ignorovat forwarding, ktery pridava www nebo https: nebo I cokoliv mimo domenu. TODO: Forwarding na LEGALNI dmenu…</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Když je velikost stránky příliš malá na kvalitní web</t>
-  </si>
-  <si>
-    <t>Links</t>
-  </si>
-  <si>
     <t>Obsahuje odkazy na oficialni web či adresu oficiálního vlastníka OZ</t>
   </si>
   <si>
@@ -181,27 +168,12 @@
     <t>Frames</t>
   </si>
   <si>
-    <t>Přiliš mnoho frames... Casto znaci reklamy...</t>
-  </si>
-  <si>
-    <t>Suspicios URL. Www neco, obsahuje OZ a potom spoustu dalsich znaku apod.</t>
-  </si>
-  <si>
     <t>SKeywords</t>
   </si>
   <si>
-    <t>Uvodni stranka obsahuje OZ konkurence</t>
-  </si>
-  <si>
-    <t>myskoda</t>
-  </si>
-  <si>
     <t>Gowner</t>
   </si>
   <si>
-    <t>Dobrý vlastník domeny. Obsahuje v ownerovi OZ</t>
-  </si>
-  <si>
     <t>Toto maji byt stejni owneri</t>
   </si>
   <si>
@@ -214,9 +186,6 @@
     <t>Bforward</t>
   </si>
   <si>
-    <t>Spatny forward na stranky konkurence nebo nekoho spatneho…</t>
-  </si>
-  <si>
     <t>Scontent</t>
   </si>
   <si>
@@ -232,26 +201,135 @@
     <t>Blinks</t>
   </si>
   <si>
-    <t>stranka obsahuje odkazy na stranky, oznacene jako BAD</t>
-  </si>
-  <si>
     <t>info-skoda-auto.sk skoda-auto-web.cz skoda-club.cz servisskoda, servis-skoda skodadily skodahome skodalevne skodaleasing skodaslevy skodateam portalskoda skodaweb</t>
   </si>
   <si>
-    <t>e-skoda.cz eshopskoda.cz eskoda-shop.cz mercedesshop.com svetskoda</t>
-  </si>
-  <si>
-    <t>skoda-auto na auto-skoda wwwskoda</t>
+    <t>Sowner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlastnik je proflaknutz podvodnik, tj. ma vice domen, ktere jsou marknute jako BAD autoklub-skoda.cz  clubskoda.cz skodafoto.cz </t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>GLinks</t>
+  </si>
+  <si>
+    <t>Opravdovy zkudce - je u nej zamer na cizi IZ vydelat (parkuje, dava jako ze pekny obsah, ale ma reklamy apod)</t>
+  </si>
+  <si>
+    <t>Maji busness ale kompetne provazene (zameruji se na ruzne I konkurencni znacky a provazuji dokupy), tam je zamer prolinkovat, tezke odstranit</t>
+  </si>
+  <si>
+    <t>Maji svuj business, ale rozsirili nabidku o konkurenci, jedna se spise o omyl (lehke odstranit)</t>
+  </si>
+  <si>
+    <t>Yneuyiti pro vlastni propagaci (tedy ne zisk)</t>
+  </si>
+  <si>
+    <t>NoOz</t>
+  </si>
+  <si>
+    <t>Skutencz vlastnik ma reklamu na konkurenci???</t>
+  </si>
+  <si>
+    <t>e-skoda.cz eshopskoda.cz eskoda-shop.cz mercedesshop.com svetskoda nd-renault.cz renaultlevne.cz renaultnahradnidily renaultlaguna.cz renaultservis renaultweb</t>
+  </si>
+  <si>
+    <t>Privydelat reklamou roydil oproti cilenemu parazitovani</t>
+  </si>
+  <si>
+    <t>Co treba klubz&lt; maji reklamu a tak je to v cajku&lt;</t>
+  </si>
+  <si>
+    <t>thalia-renault.cz  mercedescars.cz  mercedesforum.cz  mercedeslevne.cz  citroen-berlingo.cz  portal-citroen.cz  dilycitroen.cz  citroenstore.cz  citroenweb.cz  citroenbrno.cz</t>
+  </si>
+  <si>
+    <t>Doména existuje, ale nejdou stáhnout žádné stránky, jinými slovy na webu neni žádný obsah.</t>
+  </si>
+  <si>
+    <t>Když se jedná o doménu, která obsahuje webove stranky providera nebo se na strankách pracuje, nebo i forward na defaultní PARK stránku poskytovatele webu</t>
+  </si>
+  <si>
+    <t>Je tam forwarding mimo doménu, tj. forwarduje se na jinou doménu.</t>
+  </si>
+  <si>
+    <t>Když je velikost stránky příliš malá na kvalitní web, v tuto chvíli menší než 4000 bytů.</t>
+  </si>
+  <si>
+    <t>Suspicios URL. Patern WWW?, obsahuje OZ ale k tomu spoustu dalsich znaku apod.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Přiliš mnoho frames.. (více jak 2). Casto znaci reklamy... </t>
+  </si>
+  <si>
+    <t>Uvodni stranka obsahuje OZ konkurence, sex, porno, kasino, slova, která nepatří do oboru Oz (třeba pro auta je to ubytování apod.)</t>
+  </si>
+  <si>
+    <t>Dobrý vlastník domeny- owner domény obsahuje OZ</t>
+  </si>
+  <si>
+    <t>Forward na stranky konkurence nebo na stranky, které jsou již označené jako BAD.</t>
+  </si>
+  <si>
+    <t>Stranka obsahuje odkazy na stranky, oznacene jako BAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zatím není funkční - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bmwlevne.cz bmw-olomouc.cz hyundaisantafe.cz   hyundaicz.cz hyundaiweb.cz  hyundaiix35.cz   hyundailevne.cz   portal-honda.cz   hondaclub.cz hondalevne.cz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nahradnidilyhonda.cz  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hondaweb.cz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">myskoda peugeotcentrum.cz peugeot-auta, peugeot-auta peugeotweb.cz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">skoda-auto na auto-skoda wwwskoda peugeotlevne.cz peugeot-shop.cz tvujpeugeot.cz </t>
+  </si>
+  <si>
+    <t>All domains</t>
+  </si>
+  <si>
+    <t>CZ domains</t>
+  </si>
+  <si>
+    <t>CZ domains existed</t>
+  </si>
+  <si>
+    <t>All OZ</t>
+  </si>
+  <si>
+    <t>UPV</t>
+  </si>
+  <si>
+    <t>OHIM</t>
+  </si>
+  <si>
+    <t>No duplicated UPV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00"/>
+    <numFmt numFmtId="165" formatCode="#\ ###\ ###"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,19 +345,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -317,10 +382,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,7 +706,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -647,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -661,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -669,10 +736,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -680,10 +747,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -691,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -702,10 +769,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -713,10 +780,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -724,10 +791,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -735,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -746,10 +813,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -757,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -768,10 +835,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -779,10 +846,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -790,10 +857,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -801,10 +868,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -812,21 +879,33 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2">
@@ -973,47 +1052,61 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:4">
       <c r="B49" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
       <c r="C50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
       <c r="C51" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="2:3">
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
       <c r="C52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3">
+        <v>21</v>
+      </c>
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
       <c r="B55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
       <c r="B57" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1025,24 +1118,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1873392</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3">
+        <v>568272</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2/B1</f>
+        <v>0.30333854313459224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="3">
+        <v>467953</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3/B2</f>
+        <v>0.82346657938452006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3">
+        <v>556969</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3">
+        <v>52479</v>
+      </c>
+      <c r="C6" s="4">
+        <f>B6/B5</f>
+        <v>9.4222479168499504E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="3">
+        <v>48267</v>
+      </c>
+      <c r="C7" s="4">
+        <f>B7/B5</f>
+        <v>8.6660119324414822E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="3">
+        <v>504490</v>
+      </c>
+      <c r="C8" s="4">
+        <f>B8/B5</f>
+        <v>0.90577752083150054</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>